<commit_message>
develop-payroll:fix nip in template for penghasilan tidak teratur
</commit_message>
<xml_diff>
--- a/public/template_penghasilan_tidak_teratur-pengganti_biaya_kesehatan.xlsx
+++ b/public/template_penghasilan_tidak_teratur-pengganti_biaya_kesehatan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\hcs\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okann\OneDrive\Dokumen\GitHub\hcs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418E248E-A73C-4764-BD0E-B434728A83B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7944"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,30 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="1153">
-  <si>
-    <t>00102</t>
-  </si>
-  <si>
-    <t>00105</t>
-  </si>
-  <si>
-    <t>00107</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="1162">
   <si>
     <t>00110</t>
   </si>
@@ -140,18 +123,9 @@
     <t>00210</t>
   </si>
   <si>
-    <t>00216</t>
-  </si>
-  <si>
     <t>00218</t>
   </si>
   <si>
-    <t>00221</t>
-  </si>
-  <si>
-    <t>00224</t>
-  </si>
-  <si>
     <t>00227</t>
   </si>
   <si>
@@ -164,9 +138,6 @@
     <t>00234</t>
   </si>
   <si>
-    <t>00235</t>
-  </si>
-  <si>
     <t>00236</t>
   </si>
   <si>
@@ -269,9 +240,6 @@
     <t>00314</t>
   </si>
   <si>
-    <t>00315</t>
-  </si>
-  <si>
     <t>00316</t>
   </si>
   <si>
@@ -281,9 +249,6 @@
     <t>00320</t>
   </si>
   <si>
-    <t>00321</t>
-  </si>
-  <si>
     <t>00324</t>
   </si>
   <si>
@@ -326,9 +291,6 @@
     <t>00349</t>
   </si>
   <si>
-    <t>00351</t>
-  </si>
-  <si>
     <t>00353</t>
   </si>
   <si>
@@ -470,12 +432,6 @@
     <t>00459</t>
   </si>
   <si>
-    <t>00462</t>
-  </si>
-  <si>
-    <t>00463</t>
-  </si>
-  <si>
     <t>00464</t>
   </si>
   <si>
@@ -644,9 +600,6 @@
     <t>00551</t>
   </si>
   <si>
-    <t>00552</t>
-  </si>
-  <si>
     <t>00558</t>
   </si>
   <si>
@@ -821,9 +774,6 @@
     <t>00630</t>
   </si>
   <si>
-    <t>00631</t>
-  </si>
-  <si>
     <t>00632</t>
   </si>
   <si>
@@ -1139,9 +1089,6 @@
     <t>00790</t>
   </si>
   <si>
-    <t>00791</t>
-  </si>
-  <si>
     <t>00793</t>
   </si>
   <si>
@@ -1154,9 +1101,6 @@
     <t>00797</t>
   </si>
   <si>
-    <t>00798</t>
-  </si>
-  <si>
     <t>00800</t>
   </si>
   <si>
@@ -1241,9 +1185,6 @@
     <t>00839</t>
   </si>
   <si>
-    <t>00840</t>
-  </si>
-  <si>
     <t>00842</t>
   </si>
   <si>
@@ -1295,9 +1236,6 @@
     <t>00867</t>
   </si>
   <si>
-    <t>00873</t>
-  </si>
-  <si>
     <t>00874</t>
   </si>
   <si>
@@ -1325,9 +1263,6 @@
     <t>00883</t>
   </si>
   <si>
-    <t>00885</t>
-  </si>
-  <si>
     <t>00891</t>
   </si>
   <si>
@@ -1352,12 +1287,6 @@
     <t>00906</t>
   </si>
   <si>
-    <t>00907</t>
-  </si>
-  <si>
-    <t>00908</t>
-  </si>
-  <si>
     <t>00910</t>
   </si>
   <si>
@@ -1412,9 +1341,6 @@
     <t>00942</t>
   </si>
   <si>
-    <t>00945</t>
-  </si>
-  <si>
     <t>00946</t>
   </si>
   <si>
@@ -1766,9 +1692,6 @@
     <t>01097</t>
   </si>
   <si>
-    <t>01098</t>
-  </si>
-  <si>
     <t>01099</t>
   </si>
   <si>
@@ -1832,9 +1755,6 @@
     <t>01124</t>
   </si>
   <si>
-    <t>01125</t>
-  </si>
-  <si>
     <t>01126</t>
   </si>
   <si>
@@ -2081,9 +2001,6 @@
     <t>01227</t>
   </si>
   <si>
-    <t>01228</t>
-  </si>
-  <si>
     <t>01231</t>
   </si>
   <si>
@@ -2180,9 +2097,6 @@
     <t>01269</t>
   </si>
   <si>
-    <t>01270</t>
-  </si>
-  <si>
     <t>01271</t>
   </si>
   <si>
@@ -2255,9 +2169,6 @@
     <t>01298</t>
   </si>
   <si>
-    <t>01299</t>
-  </si>
-  <si>
     <t>01300</t>
   </si>
   <si>
@@ -2540,9 +2451,6 @@
     <t>01403</t>
   </si>
   <si>
-    <t>01404</t>
-  </si>
-  <si>
     <t>01405</t>
   </si>
   <si>
@@ -2816,9 +2724,6 @@
     <t>01498</t>
   </si>
   <si>
-    <t>01499</t>
-  </si>
-  <si>
     <t>01500</t>
   </si>
   <si>
@@ -2849,9 +2754,6 @@
     <t>01509</t>
   </si>
   <si>
-    <t>01510</t>
-  </si>
-  <si>
     <t>01511</t>
   </si>
   <si>
@@ -2876,168 +2778,33 @@
     <t>X1094</t>
   </si>
   <si>
-    <t>X1123</t>
-  </si>
-  <si>
-    <t>X1197</t>
-  </si>
-  <si>
-    <t>X1198</t>
-  </si>
-  <si>
-    <t>X1199</t>
-  </si>
-  <si>
-    <t>X1200</t>
-  </si>
-  <si>
-    <t>X1201</t>
-  </si>
-  <si>
-    <t>X1202</t>
-  </si>
-  <si>
-    <t>X1203</t>
-  </si>
-  <si>
-    <t>X1204</t>
-  </si>
-  <si>
-    <t>X1206</t>
-  </si>
-  <si>
-    <t>X1208</t>
-  </si>
-  <si>
-    <t>X1209</t>
-  </si>
-  <si>
-    <t>X1210</t>
-  </si>
-  <si>
     <t>X1211</t>
   </si>
   <si>
     <t>X1212</t>
   </si>
   <si>
-    <t>X1213</t>
-  </si>
-  <si>
-    <t>X1215</t>
-  </si>
-  <si>
-    <t>X1216</t>
-  </si>
-  <si>
-    <t>X1217</t>
-  </si>
-  <si>
-    <t>X1218</t>
-  </si>
-  <si>
-    <t>X1219</t>
-  </si>
-  <si>
     <t>X1220</t>
   </si>
   <si>
-    <t>X1222</t>
-  </si>
-  <si>
-    <t>X1223</t>
-  </si>
-  <si>
     <t>X1224</t>
   </si>
   <si>
-    <t>X1225</t>
-  </si>
-  <si>
-    <t>X1226</t>
-  </si>
-  <si>
-    <t>X1227</t>
-  </si>
-  <si>
-    <t>X1228</t>
-  </si>
-  <si>
-    <t>X1229</t>
-  </si>
-  <si>
-    <t>X1230</t>
-  </si>
-  <si>
     <t>X1231</t>
   </si>
   <si>
-    <t>X1232</t>
-  </si>
-  <si>
-    <t>X1233</t>
-  </si>
-  <si>
-    <t>X1234</t>
-  </si>
-  <si>
     <t>X1235</t>
   </si>
   <si>
-    <t>X1236</t>
-  </si>
-  <si>
-    <t>X1237</t>
-  </si>
-  <si>
-    <t>X1238</t>
-  </si>
-  <si>
-    <t>X1240</t>
-  </si>
-  <si>
-    <t>X1241</t>
-  </si>
-  <si>
-    <t>X1243</t>
-  </si>
-  <si>
     <t>X1244</t>
   </si>
   <si>
-    <t>X1245</t>
-  </si>
-  <si>
-    <t>X1246</t>
-  </si>
-  <si>
-    <t>X1247</t>
-  </si>
-  <si>
-    <t>X1248</t>
-  </si>
-  <si>
-    <t>X1249</t>
-  </si>
-  <si>
     <t>X1250</t>
   </si>
   <si>
-    <t>X1251</t>
-  </si>
-  <si>
     <t>X1252</t>
   </si>
   <si>
-    <t>X1253</t>
-  </si>
-  <si>
-    <t>X1254</t>
-  </si>
-  <si>
-    <t>X1255</t>
-  </si>
-  <si>
     <t>X1257</t>
   </si>
   <si>
@@ -3167,9 +2934,6 @@
     <t>X1301</t>
   </si>
   <si>
-    <t>X1302</t>
-  </si>
-  <si>
     <t>X1304</t>
   </si>
   <si>
@@ -3383,9 +3147,6 @@
     <t>X1376</t>
   </si>
   <si>
-    <t>x666</t>
-  </si>
-  <si>
     <t>XX006</t>
   </si>
   <si>
@@ -3443,39 +3204,18 @@
     <t>ZZ003</t>
   </si>
   <si>
-    <t>ZZ004</t>
-  </si>
-  <si>
     <t>ZZ006</t>
   </si>
   <si>
     <t>ZZ009</t>
   </si>
   <si>
-    <t>ZZ012</t>
-  </si>
-  <si>
-    <t>ZZ013</t>
-  </si>
-  <si>
-    <t>ZZ020</t>
-  </si>
-  <si>
     <t>ZZ021</t>
   </si>
   <si>
     <t>ZZ022</t>
   </si>
   <si>
-    <t>ZZ023</t>
-  </si>
-  <si>
-    <t>ZZ024</t>
-  </si>
-  <si>
-    <t>ZZ025</t>
-  </si>
-  <si>
     <t>ZZ026</t>
   </si>
   <si>
@@ -3492,12 +3232,291 @@
   </si>
   <si>
     <t>Keterangan</t>
+  </si>
+  <si>
+    <t>01515</t>
+  </si>
+  <si>
+    <t>01516</t>
+  </si>
+  <si>
+    <t>01517</t>
+  </si>
+  <si>
+    <t>01518</t>
+  </si>
+  <si>
+    <t>01519</t>
+  </si>
+  <si>
+    <t>01520</t>
+  </si>
+  <si>
+    <t>01521</t>
+  </si>
+  <si>
+    <t>01522</t>
+  </si>
+  <si>
+    <t>01523</t>
+  </si>
+  <si>
+    <t>01524</t>
+  </si>
+  <si>
+    <t>01525</t>
+  </si>
+  <si>
+    <t>01526</t>
+  </si>
+  <si>
+    <t>01527</t>
+  </si>
+  <si>
+    <t>01528</t>
+  </si>
+  <si>
+    <t>01529</t>
+  </si>
+  <si>
+    <t>01530</t>
+  </si>
+  <si>
+    <t>01531</t>
+  </si>
+  <si>
+    <t>01532</t>
+  </si>
+  <si>
+    <t>01533</t>
+  </si>
+  <si>
+    <t>01534</t>
+  </si>
+  <si>
+    <t>01535</t>
+  </si>
+  <si>
+    <t>01536</t>
+  </si>
+  <si>
+    <t>01537</t>
+  </si>
+  <si>
+    <t>01538</t>
+  </si>
+  <si>
+    <t>01539</t>
+  </si>
+  <si>
+    <t>01540</t>
+  </si>
+  <si>
+    <t>01541</t>
+  </si>
+  <si>
+    <t>01542</t>
+  </si>
+  <si>
+    <t>01543</t>
+  </si>
+  <si>
+    <t>01544</t>
+  </si>
+  <si>
+    <t>01545</t>
+  </si>
+  <si>
+    <t>01546</t>
+  </si>
+  <si>
+    <t>01547</t>
+  </si>
+  <si>
+    <t>01548</t>
+  </si>
+  <si>
+    <t>01549</t>
+  </si>
+  <si>
+    <t>01550</t>
+  </si>
+  <si>
+    <t>01551</t>
+  </si>
+  <si>
+    <t>01552</t>
+  </si>
+  <si>
+    <t>01553</t>
+  </si>
+  <si>
+    <t>01554</t>
+  </si>
+  <si>
+    <t>01555</t>
+  </si>
+  <si>
+    <t>01556</t>
+  </si>
+  <si>
+    <t>01557</t>
+  </si>
+  <si>
+    <t>Dolore eius voluptat</t>
+  </si>
+  <si>
+    <t>X1378</t>
+  </si>
+  <si>
+    <t>X1379</t>
+  </si>
+  <si>
+    <t>X1380</t>
+  </si>
+  <si>
+    <t>X1381</t>
+  </si>
+  <si>
+    <t>X1382</t>
+  </si>
+  <si>
+    <t>X1383</t>
+  </si>
+  <si>
+    <t>X1384</t>
+  </si>
+  <si>
+    <t>X1385</t>
+  </si>
+  <si>
+    <t>X1386</t>
+  </si>
+  <si>
+    <t>X1387</t>
+  </si>
+  <si>
+    <t>X1388</t>
+  </si>
+  <si>
+    <t>X1389</t>
+  </si>
+  <si>
+    <t>X1390</t>
+  </si>
+  <si>
+    <t>X1391</t>
+  </si>
+  <si>
+    <t>X1392</t>
+  </si>
+  <si>
+    <t>X1393</t>
+  </si>
+  <si>
+    <t>X1394</t>
+  </si>
+  <si>
+    <t>X1395</t>
+  </si>
+  <si>
+    <t>X1396</t>
+  </si>
+  <si>
+    <t>X1397</t>
+  </si>
+  <si>
+    <t>X1398</t>
+  </si>
+  <si>
+    <t>X1399</t>
+  </si>
+  <si>
+    <t>X1400</t>
+  </si>
+  <si>
+    <t>X1401</t>
+  </si>
+  <si>
+    <t>X1402</t>
+  </si>
+  <si>
+    <t>X1403</t>
+  </si>
+  <si>
+    <t>X1404</t>
+  </si>
+  <si>
+    <t>X1405</t>
+  </si>
+  <si>
+    <t>X1406</t>
+  </si>
+  <si>
+    <t>X1407</t>
+  </si>
+  <si>
+    <t>X1408</t>
+  </si>
+  <si>
+    <t>X1409</t>
+  </si>
+  <si>
+    <t>X1410</t>
+  </si>
+  <si>
+    <t>X1411</t>
+  </si>
+  <si>
+    <t>X1412</t>
+  </si>
+  <si>
+    <t>X1413</t>
+  </si>
+  <si>
+    <t>X1414</t>
+  </si>
+  <si>
+    <t>X1415</t>
+  </si>
+  <si>
+    <t>X1416</t>
+  </si>
+  <si>
+    <t>X1417</t>
+  </si>
+  <si>
+    <t>X1418</t>
+  </si>
+  <si>
+    <t>X1419</t>
+  </si>
+  <si>
+    <t>X1420</t>
+  </si>
+  <si>
+    <t>X1421</t>
+  </si>
+  <si>
+    <t>X1422</t>
+  </si>
+  <si>
+    <t>ZZ029</t>
+  </si>
+  <si>
+    <t>ZZ030</t>
+  </si>
+  <si>
+    <t>ZZ031</t>
+  </si>
+  <si>
+    <t>ZZ032</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3842,24 +3861,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1151"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1150</v>
+        <v>1066</v>
       </c>
       <c r="B1" t="s">
-        <v>1151</v>
+        <v>1067</v>
       </c>
       <c r="C1" t="s">
-        <v>1152</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -8429,1187 +8448,1237 @@
     </row>
     <row r="915" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A915" t="s">
-        <v>913</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="916" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A916" t="s">
-        <v>914</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="917" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A917" t="s">
-        <v>915</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="918" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A918" t="s">
-        <v>916</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="919" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A919" t="s">
-        <v>917</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="920" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
-        <v>918</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="921" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A921" t="s">
-        <v>919</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="922" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A922" t="s">
-        <v>920</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="923" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A923" t="s">
-        <v>921</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="924" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A924" t="s">
-        <v>922</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="925" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
-        <v>923</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="926" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A926" t="s">
-        <v>924</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="927" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A927" t="s">
-        <v>925</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="928" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A928" t="s">
-        <v>926</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="929" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A929" t="s">
-        <v>927</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="930" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A930" t="s">
-        <v>928</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="931" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A931" t="s">
-        <v>929</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="932" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A932" t="s">
-        <v>930</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="933" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A933" t="s">
-        <v>931</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="934" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A934" t="s">
-        <v>932</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="935" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A935" t="s">
-        <v>933</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="936" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A936" t="s">
-        <v>934</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="937" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A937" t="s">
-        <v>935</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="938" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A938" t="s">
-        <v>936</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="939" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A939" t="s">
-        <v>937</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="940" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A940" t="s">
-        <v>938</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="941" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A941" t="s">
-        <v>939</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="942" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
-        <v>940</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="943" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A943" t="s">
-        <v>941</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="944" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A944" t="s">
-        <v>942</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="945" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A945" t="s">
-        <v>943</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="946" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A946" t="s">
-        <v>944</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="947" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A947" t="s">
-        <v>945</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="948" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A948" t="s">
-        <v>946</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="949" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A949" t="s">
-        <v>947</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="950" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A950" t="s">
-        <v>948</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="951" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A951" t="s">
-        <v>949</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="952" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A952" t="s">
-        <v>950</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="953" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A953" t="s">
-        <v>951</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="954" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A954" t="s">
-        <v>952</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="955" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A955" t="s">
-        <v>953</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="956" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A956" t="s">
-        <v>954</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="957" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A957" t="s">
-        <v>955</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="958" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A958" t="s">
-        <v>956</v>
+      <c r="A958">
+        <v>123123</v>
       </c>
     </row>
     <row r="959" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A959" t="s">
-        <v>957</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="960" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A960" t="s">
-        <v>958</v>
+        <v>913</v>
       </c>
     </row>
     <row r="961" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A961" t="s">
-        <v>959</v>
+        <v>914</v>
       </c>
     </row>
     <row r="962" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A962" t="s">
-        <v>960</v>
+        <v>915</v>
       </c>
     </row>
     <row r="963" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A963" t="s">
-        <v>961</v>
+        <v>916</v>
       </c>
     </row>
     <row r="964" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A964" t="s">
-        <v>962</v>
+        <v>917</v>
       </c>
     </row>
     <row r="965" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A965" t="s">
-        <v>963</v>
+        <v>918</v>
       </c>
     </row>
     <row r="966" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A966" t="s">
-        <v>964</v>
+        <v>919</v>
       </c>
     </row>
     <row r="967" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A967" t="s">
-        <v>965</v>
+        <v>920</v>
       </c>
     </row>
     <row r="968" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A968" t="s">
-        <v>966</v>
+        <v>921</v>
       </c>
     </row>
     <row r="969" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A969" t="s">
-        <v>967</v>
+        <v>922</v>
       </c>
     </row>
     <row r="970" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A970" t="s">
-        <v>968</v>
+        <v>923</v>
       </c>
     </row>
     <row r="971" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A971" t="s">
-        <v>969</v>
+        <v>924</v>
       </c>
     </row>
     <row r="972" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A972" t="s">
-        <v>970</v>
+        <v>925</v>
       </c>
     </row>
     <row r="973" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A973" t="s">
-        <v>971</v>
+        <v>926</v>
       </c>
     </row>
     <row r="974" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A974" t="s">
-        <v>972</v>
+        <v>927</v>
       </c>
     </row>
     <row r="975" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A975" t="s">
-        <v>973</v>
+        <v>928</v>
       </c>
     </row>
     <row r="976" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A976" t="s">
-        <v>974</v>
+        <v>929</v>
       </c>
     </row>
     <row r="977" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A977" t="s">
-        <v>975</v>
+        <v>930</v>
       </c>
     </row>
     <row r="978" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A978" t="s">
-        <v>976</v>
+        <v>931</v>
       </c>
     </row>
     <row r="979" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A979" t="s">
-        <v>977</v>
+        <v>932</v>
       </c>
     </row>
     <row r="980" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A980" t="s">
-        <v>978</v>
+        <v>933</v>
       </c>
     </row>
     <row r="981" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A981" t="s">
-        <v>979</v>
+        <v>934</v>
       </c>
     </row>
     <row r="982" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A982" t="s">
-        <v>980</v>
+        <v>935</v>
       </c>
     </row>
     <row r="983" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A983" t="s">
-        <v>981</v>
+        <v>936</v>
       </c>
     </row>
     <row r="984" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A984" t="s">
-        <v>982</v>
+        <v>937</v>
       </c>
     </row>
     <row r="985" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A985" t="s">
-        <v>983</v>
+        <v>938</v>
       </c>
     </row>
     <row r="986" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A986" t="s">
-        <v>984</v>
+        <v>939</v>
       </c>
     </row>
     <row r="987" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A987" t="s">
-        <v>985</v>
+        <v>940</v>
       </c>
     </row>
     <row r="988" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A988" t="s">
-        <v>986</v>
+        <v>941</v>
       </c>
     </row>
     <row r="989" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A989" t="s">
-        <v>987</v>
+        <v>942</v>
       </c>
     </row>
     <row r="990" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A990" t="s">
-        <v>988</v>
+        <v>943</v>
       </c>
     </row>
     <row r="991" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A991" t="s">
-        <v>989</v>
+        <v>944</v>
       </c>
     </row>
     <row r="992" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A992" t="s">
-        <v>990</v>
+        <v>945</v>
       </c>
     </row>
     <row r="993" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A993" t="s">
-        <v>991</v>
+        <v>946</v>
       </c>
     </row>
     <row r="994" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A994" t="s">
-        <v>992</v>
+        <v>947</v>
       </c>
     </row>
     <row r="995" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A995" t="s">
-        <v>993</v>
+        <v>948</v>
       </c>
     </row>
     <row r="996" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A996" t="s">
-        <v>994</v>
+        <v>949</v>
       </c>
     </row>
     <row r="997" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A997" t="s">
-        <v>995</v>
+        <v>950</v>
       </c>
     </row>
     <row r="998" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A998" t="s">
-        <v>996</v>
+        <v>951</v>
       </c>
     </row>
     <row r="999" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A999" t="s">
-        <v>997</v>
+        <v>952</v>
       </c>
     </row>
     <row r="1000" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1000" t="s">
-        <v>998</v>
+        <v>953</v>
       </c>
     </row>
     <row r="1001" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1001" t="s">
-        <v>999</v>
+        <v>954</v>
       </c>
     </row>
     <row r="1002" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1002" t="s">
-        <v>1000</v>
+        <v>955</v>
       </c>
     </row>
     <row r="1003" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1003" t="s">
-        <v>1001</v>
+        <v>956</v>
       </c>
     </row>
     <row r="1004" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1004" t="s">
-        <v>1002</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1005" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1005" t="s">
-        <v>1003</v>
+        <v>958</v>
       </c>
     </row>
     <row r="1006" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1006" t="s">
-        <v>1004</v>
+        <v>959</v>
       </c>
     </row>
     <row r="1007" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1007" t="s">
-        <v>1005</v>
+        <v>960</v>
       </c>
     </row>
     <row r="1008" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1008" t="s">
-        <v>1006</v>
+        <v>961</v>
       </c>
     </row>
     <row r="1009" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1009" t="s">
-        <v>1007</v>
+        <v>962</v>
       </c>
     </row>
     <row r="1010" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1010" t="s">
-        <v>1008</v>
+        <v>963</v>
       </c>
     </row>
     <row r="1011" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1011" t="s">
-        <v>1009</v>
+        <v>964</v>
       </c>
     </row>
     <row r="1012" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1012" t="s">
-        <v>1010</v>
+        <v>965</v>
       </c>
     </row>
     <row r="1013" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1013" t="s">
-        <v>1011</v>
+        <v>966</v>
       </c>
     </row>
     <row r="1014" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1014" t="s">
-        <v>1012</v>
+        <v>967</v>
       </c>
     </row>
     <row r="1015" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1015" t="s">
-        <v>1013</v>
+        <v>968</v>
       </c>
     </row>
     <row r="1016" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1016" t="s">
-        <v>1014</v>
+        <v>969</v>
       </c>
     </row>
     <row r="1017" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1017" t="s">
-        <v>1015</v>
+        <v>970</v>
       </c>
     </row>
     <row r="1018" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1018" t="s">
-        <v>1016</v>
+        <v>971</v>
       </c>
     </row>
     <row r="1019" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1019" t="s">
-        <v>1017</v>
+        <v>972</v>
       </c>
     </row>
     <row r="1020" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1020" t="s">
-        <v>1018</v>
+        <v>973</v>
       </c>
     </row>
     <row r="1021" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1021" t="s">
-        <v>1019</v>
+        <v>974</v>
       </c>
     </row>
     <row r="1022" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1022" t="s">
-        <v>1020</v>
+        <v>975</v>
       </c>
     </row>
     <row r="1023" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1023" t="s">
-        <v>1021</v>
+        <v>976</v>
       </c>
     </row>
     <row r="1024" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1024" t="s">
-        <v>1022</v>
+        <v>977</v>
       </c>
     </row>
     <row r="1025" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1025" t="s">
-        <v>1023</v>
+        <v>978</v>
       </c>
     </row>
     <row r="1026" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1026" t="s">
-        <v>1024</v>
+        <v>979</v>
       </c>
     </row>
     <row r="1027" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1027" t="s">
-        <v>1025</v>
+        <v>980</v>
       </c>
     </row>
     <row r="1028" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1028" t="s">
-        <v>1026</v>
+        <v>981</v>
       </c>
     </row>
     <row r="1029" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1029" t="s">
-        <v>1027</v>
+        <v>982</v>
       </c>
     </row>
     <row r="1030" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1030" t="s">
-        <v>1028</v>
+        <v>983</v>
       </c>
     </row>
     <row r="1031" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1031" t="s">
-        <v>1029</v>
+        <v>984</v>
       </c>
     </row>
     <row r="1032" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1032" t="s">
-        <v>1030</v>
+        <v>985</v>
       </c>
     </row>
     <row r="1033" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1033" t="s">
-        <v>1031</v>
+        <v>986</v>
       </c>
     </row>
     <row r="1034" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1034" t="s">
-        <v>1032</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1035" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1035" t="s">
-        <v>1033</v>
+        <v>988</v>
       </c>
     </row>
     <row r="1036" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1036" t="s">
-        <v>1034</v>
+        <v>989</v>
       </c>
     </row>
     <row r="1037" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1037" t="s">
-        <v>1035</v>
+        <v>990</v>
       </c>
     </row>
     <row r="1038" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1038" t="s">
-        <v>1036</v>
+        <v>991</v>
       </c>
     </row>
     <row r="1039" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1039" t="s">
-        <v>1037</v>
+        <v>992</v>
       </c>
     </row>
     <row r="1040" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1040" t="s">
-        <v>1038</v>
+        <v>993</v>
       </c>
     </row>
     <row r="1041" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1041" t="s">
-        <v>1039</v>
+        <v>994</v>
       </c>
     </row>
     <row r="1042" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1042" t="s">
-        <v>1040</v>
+        <v>995</v>
       </c>
     </row>
     <row r="1043" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1043" t="s">
-        <v>1041</v>
+        <v>996</v>
       </c>
     </row>
     <row r="1044" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1044" t="s">
-        <v>1042</v>
+        <v>997</v>
       </c>
     </row>
     <row r="1045" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1045" t="s">
-        <v>1043</v>
+        <v>998</v>
       </c>
     </row>
     <row r="1046" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1046" t="s">
-        <v>1044</v>
+        <v>999</v>
       </c>
     </row>
     <row r="1047" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1047" t="s">
-        <v>1045</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="1048" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1048" t="s">
-        <v>1046</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1049" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1049" t="s">
-        <v>1047</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="1050" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1050" t="s">
-        <v>1048</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="1051" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1051" t="s">
-        <v>1049</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="1052" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1052" t="s">
-        <v>1050</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="1053" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1053" t="s">
-        <v>1051</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="1054" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1054" t="s">
-        <v>1052</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="1055" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1055" t="s">
-        <v>1053</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="1056" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1056" t="s">
-        <v>1054</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="1057" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1057" t="s">
-        <v>1055</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="1058" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1058" t="s">
-        <v>1056</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="1059" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1059" t="s">
-        <v>1057</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="1060" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1060" t="s">
-        <v>1058</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="1061" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1061" t="s">
-        <v>1059</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="1062" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1062" t="s">
-        <v>1060</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="1063" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1063" t="s">
-        <v>1061</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="1064" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1064" t="s">
-        <v>1062</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="1065" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1065" t="s">
-        <v>1063</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="1066" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1066" t="s">
-        <v>1064</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="1067" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1067" t="s">
-        <v>1065</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="1068" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1068" t="s">
-        <v>1066</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="1069" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1069" t="s">
-        <v>1067</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="1070" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1070" t="s">
-        <v>1068</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="1071" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1071" t="s">
-        <v>1069</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="1072" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1072" t="s">
-        <v>1070</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="1073" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1073" t="s">
-        <v>1071</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="1074" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1074" t="s">
-        <v>1072</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="1075" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1075" t="s">
-        <v>1073</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="1076" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1076" t="s">
-        <v>1074</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="1077" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1077" t="s">
-        <v>1075</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="1078" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1078" t="s">
-        <v>1076</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="1079" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1079" t="s">
-        <v>1077</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="1080" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1080" t="s">
-        <v>1078</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="1081" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1081" t="s">
-        <v>1079</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="1082" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1082" t="s">
-        <v>1080</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="1083" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1083" t="s">
-        <v>1081</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="1084" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1084" t="s">
-        <v>1082</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="1085" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1085" t="s">
-        <v>1083</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="1086" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1086" t="s">
-        <v>1084</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="1087" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1087" t="s">
-        <v>1085</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1088" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1088" t="s">
-        <v>1086</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="1089" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1089" t="s">
-        <v>1087</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="1090" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1090" t="s">
-        <v>1088</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1091" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1091" t="s">
-        <v>1089</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1092" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1092" t="s">
-        <v>1090</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1093" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1093" t="s">
-        <v>1091</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1094" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1094" t="s">
-        <v>1092</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1095" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1095" t="s">
-        <v>1093</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1096" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1096" t="s">
-        <v>1094</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1097" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1097" t="s">
-        <v>1095</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1098" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1098" t="s">
-        <v>1096</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1099" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1099" t="s">
-        <v>1097</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1100" t="s">
-        <v>1098</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1101" t="s">
-        <v>1099</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1102" t="s">
-        <v>1100</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1103" t="s">
-        <v>1101</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1104" t="s">
-        <v>1102</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1105" t="s">
-        <v>1103</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1106" t="s">
-        <v>1104</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1107" t="s">
-        <v>1105</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1108" t="s">
-        <v>1106</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1109" t="s">
-        <v>1107</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1110" t="s">
-        <v>1108</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1111" t="s">
-        <v>1109</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1112" t="s">
-        <v>1110</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1113" t="s">
-        <v>1111</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1114" t="s">
-        <v>1112</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1115" t="s">
-        <v>1113</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="1116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1116" t="s">
-        <v>1114</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1117" t="s">
-        <v>1115</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1118" t="s">
-        <v>1116</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1119" t="s">
-        <v>1117</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1120" t="s">
-        <v>1118</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1121" t="s">
-        <v>1119</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1122" t="s">
-        <v>1120</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1123" t="s">
-        <v>1121</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1124" t="s">
-        <v>1122</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1125" t="s">
-        <v>1123</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1126" t="s">
-        <v>1124</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1127" t="s">
-        <v>1125</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1128" t="s">
-        <v>1126</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1129" t="s">
-        <v>1127</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1130" t="s">
-        <v>1128</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1131" t="s">
-        <v>1129</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1132" t="s">
-        <v>1130</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="1133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1133" t="s">
-        <v>1131</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="1134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1134" t="s">
-        <v>1132</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="1135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1135" t="s">
-        <v>1133</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="1136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1136" t="s">
-        <v>1134</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="1137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1137" t="s">
-        <v>1135</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="1138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1138" t="s">
-        <v>1136</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="1139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1139" t="s">
-        <v>1137</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="1140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1140" t="s">
-        <v>1138</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="1141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1141" t="s">
-        <v>1139</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="1142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1142" t="s">
-        <v>1140</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="1143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1143" t="s">
-        <v>1141</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="1144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1144" t="s">
-        <v>1142</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="1145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1145" t="s">
-        <v>1143</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="1146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1146" t="s">
-        <v>1144</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="1147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1147" t="s">
-        <v>1145</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="1148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1148" t="s">
-        <v>1146</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="1149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1149" t="s">
-        <v>1147</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="1150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1150" t="s">
-        <v>1148</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="1151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1151" t="s">
-        <v>1149</v>
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1152" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1153" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1154" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1155" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1156" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1157" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1158" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1159" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1160" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1161" t="s">
+        <v>1161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>